<commit_message>
bug修改 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="255">
   <si>
     <t>请求url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,599 +403,603 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>要转移的成员id,群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200, "text":"fail/群组信息数组"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":成员id数组}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,groupname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群组id，群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理群成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>要管理的成员id,群组id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!manageGroupMem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个接口是可能界面上统一增删群成员直接保存增删后成员的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone、textcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号/名称/名称全拼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号、好友账号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模糊查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找到的用户数据数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, 群信息}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看单个群信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号、新密码、确认密码、[忘记密码时不添，登陆后修改密码需添写 ]（验证码，开发模式为9999）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置消息免打扰功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置系统提示音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取系统提示音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200, "text":状态}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200, "text":"ok"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status、groupid、userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态值（1/0）、群id、用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setNotRecieveMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setSysTipVoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, "text":"ok"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, x, y, width, height, degree, file</t>
+  </si>
+  <si>
+    <t>用户id、裁剪x,y,宽、高、角度、文件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":为1就是最终上传的头像名}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app可能会有出入，另做接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取七牛token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, text:token}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存最后选择的头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,picname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,图片名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{code:0/1/-1, text:失败/成功/无参数}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取相册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!delUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!getUploadQiniuToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!getUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, targetid, type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, text:[好友位置]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取好友/群组地图坐标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交个人地理位置接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, latitude, longtitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id, 经度，纬度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, text:ok}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18，获取某人当前地理位置接口</t>
+  </si>
+  <si>
+    <t>17，提交个人地理位置接口</t>
+  </si>
+  <si>
+    <t>16，发起群聊接口</t>
+  </si>
+  <si>
+    <t>15，从群组踢出某人</t>
+  </si>
+  <si>
+    <t>14，添加人到群组</t>
+  </si>
+  <si>
+    <t>13，从我的常用联系人列表删除人的接口</t>
+  </si>
+  <si>
+    <t>12，添加人到我的常用联系人接口</t>
+  </si>
+  <si>
+    <t>11，获取group用户列表接口</t>
+  </si>
+  <si>
+    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
+  </si>
+  <si>
+    <t>9，设置群组信息接口</t>
+  </si>
+  <si>
+    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
+  </si>
+  <si>
+    <t>7，天坊公司组织结构数据接口</t>
+  </si>
+  <si>
+    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
+  </si>
+  <si>
+    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
+  </si>
+  <si>
+    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
+  </si>
+  <si>
+    <t>2，发送验证码接口，参数countrycode，mobile</t>
+  </si>
+  <si>
+    <t>1，登录接口</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!afterLogin</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!requestText</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!newPassword</t>
+  </si>
+  <si>
+    <t>friend!getMemberFriends</t>
+  </si>
+  <si>
+    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!groupList</t>
+  </si>
+  <si>
+    <t>group!groupInfo</t>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!listGroupMemebers</t>
+  </si>
+  <si>
+    <t>friend!addFriend</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend!delFriend</t>
+  </si>
+  <si>
+    <t>group!joinGroup</t>
+  </si>
+  <si>
+    <t>group!leftGroup</t>
+  </si>
+  <si>
+    <t>subLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map!getLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account, fullname, sex, position, branch, email, phone, sign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号、名称、性别、职位、部门、email、电话、个人签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、增加修改群名称接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7、修改个人设置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8、联系人接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11、返回字段说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupids, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取群组列表（我加入的和我建的）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12、群信息群列表接口返回数据增加创建者对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(仅返回id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(返回成员数据)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群组id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,groupname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,新的群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13、同时添加多个好友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9、权限功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10、添加返回所有不是好友数据的接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增listGroupMembersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14、建群小灰条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、加入、退出、转移群接口bug查找。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>要转移的成员id,群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200, "text":"fail/群组信息数组"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":成员id数组}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,groupname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群组id，群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理群成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>要管理的成员id,群组id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!manageGroupMem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>这个接口是可能界面上统一增删群成员直接保存增删后成员的。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone、textcode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查找用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号/名称/名称全拼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号、好友账号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模糊查找</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查找到的用户数据数组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1, 群信息}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看单个群信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号、新密码、确认密码、[忘记密码时不添，登陆后修改密码需添写 ]（验证码，开发模式为9999）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置消息免打扰功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置系统提示音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取系统提示音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200, "text":状态}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200, "text":"ok"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>status、groupid、userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态值（1/0）、群id、用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setNotRecieveMsg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setSysTipVoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1, "text":"ok"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, x, y, width, height, degree, file</t>
-  </si>
-  <si>
-    <t>用户id、裁剪x,y,宽、高、角度、文件。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":为1就是最终上传的头像名}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>app可能会有出入，另做接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取七牛token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1, text:token}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存最后选择的头像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,picname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,图片名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{code:0/1/-1, text:失败/成功/无参数}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取相册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除头像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!delUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!getUploadQiniuToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!getUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, targetid, type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, text:[好友位置]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身id，目标id（群组id/或好友id）,1群0好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取好友/群组地图坐标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提交个人地理位置接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, latitude, longtitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id, 经度，纬度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, text:ok}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18，获取某人当前地理位置接口</t>
-  </si>
-  <si>
-    <t>17，提交个人地理位置接口</t>
-  </si>
-  <si>
-    <t>16，发起群聊接口</t>
-  </si>
-  <si>
-    <t>15，从群组踢出某人</t>
-  </si>
-  <si>
-    <t>14，添加人到群组</t>
-  </si>
-  <si>
-    <t>13，从我的常用联系人列表删除人的接口</t>
-  </si>
-  <si>
-    <t>12，添加人到我的常用联系人接口</t>
-  </si>
-  <si>
-    <t>11，获取group用户列表接口</t>
-  </si>
-  <si>
-    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
-  </si>
-  <si>
-    <t>9，设置群组信息接口</t>
-  </si>
-  <si>
-    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
-  </si>
-  <si>
-    <t>7，天坊公司组织结构数据接口</t>
-  </si>
-  <si>
-    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
-  </si>
-  <si>
-    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
-  </si>
-  <si>
-    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
-  </si>
-  <si>
-    <t>2，发送验证码接口，参数countrycode，mobile</t>
-  </si>
-  <si>
-    <t>1，登录接口</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!afterLogin</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!requestText</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!newPassword</t>
-  </si>
-  <si>
-    <t>friend!getMemberFriends</t>
-  </si>
-  <si>
-    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!groupList</t>
-  </si>
-  <si>
-    <t>group!groupInfo</t>
-  </si>
-  <si>
-    <t>??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!listGroupMemebers</t>
-  </si>
-  <si>
-    <t>friend!addFriend</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>friend!delFriend</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!joinGroup</t>
-  </si>
-  <si>
-    <t>group!leftGroup</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>subLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map!getLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account, fullname, sex, position, branch, email, phone, sign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号、名称、性别、职位、部门、email、电话、个人签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3、增加修改群名称接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5、加入、退出、转移群接口bug查找。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7、修改个人设置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8、联系人接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10、添加返回所有不是好友数据的接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11、返回字段说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupids, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取群组列表（我加入的和我建的）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12、群信息群列表接口返回数据增加创建者对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(仅返回id)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(返回成员数据)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群组id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增listGroupMembersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整,调整群聊targetid为GID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,groupname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,新的群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13、同时添加多个好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9、权限功能。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1178,14 +1182,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1489,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1498,7 +1502,7 @@
     <col min="1" max="1" width="34.875" customWidth="1"/>
     <col min="2" max="2" width="73.875" customWidth="1"/>
     <col min="3" max="3" width="63.875" customWidth="1"/>
-    <col min="4" max="4" width="60" customWidth="1"/>
+    <col min="4" max="4" width="102.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.25" customWidth="1"/>
     <col min="6" max="6" width="81" customWidth="1"/>
     <col min="7" max="7" width="37.125" customWidth="1"/>
@@ -1528,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -1549,10 +1553,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
@@ -1569,16 +1573,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>9</v>
@@ -1621,7 +1625,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>30</v>
@@ -1654,16 +1658,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>12</v>
@@ -1676,10 +1680,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>23</v>
@@ -1694,22 +1698,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="E11" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -1718,13 +1722,13 @@
         <v>34</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>29</v>
@@ -1739,7 +1743,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>27</v>
@@ -1760,7 +1764,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>38</v>
@@ -1781,7 +1785,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>44</v>
@@ -1800,7 +1804,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>44</v>
@@ -1923,7 +1927,7 @@
         <v>70</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>203</v>
+        <v>250</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>82</v>
@@ -1942,10 +1946,10 @@
         <v>71</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>85</v>
@@ -1981,10 +1985,10 @@
         <v>77</v>
       </c>
       <c r="C26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>104</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>90</v>
@@ -1994,35 +1998,35 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>198</v>
+        <v>230</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>240</v>
+        <v>231</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>233</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="10"/>
@@ -2032,8 +2036,8 @@
       <c r="A29" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>225</v>
+      <c r="B29" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>86</v>
@@ -2042,26 +2046,26 @@
         <v>87</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>232</v>
+        <v>222</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -2092,13 +2096,13 @@
         <v>96</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>74</v>
@@ -2108,56 +2112,56 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>233</v>
+        <v>121</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>226</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>249</v>
+        <v>237</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="10"/>
@@ -2165,16 +2169,16 @@
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>74</v>
@@ -2184,38 +2188,38 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -2231,37 +2235,37 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C40" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="10"/>
@@ -2269,16 +2273,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="C42" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="10"/>
@@ -2286,36 +2290,36 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="E43" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -2331,38 +2335,38 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C47" s="12" t="s">
+      <c r="E47" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -2377,12 +2381,12 @@
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:4" ht="40.5" customHeight="1">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2410,143 +2414,143 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2557,93 +2561,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="94.5" customWidth="1"/>
+    <col min="1" max="1" width="75.875" customWidth="1"/>
     <col min="2" max="2" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="21" t="s">
-        <v>221</v>
+      <c r="A1" s="20" t="s">
+        <v>216</v>
       </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="22" t="s">
-        <v>215</v>
+      <c r="A2" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="22" t="s">
-        <v>216</v>
+      <c r="A3" s="21" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="22" t="s">
-        <v>217</v>
+      <c r="A4" s="21" t="s">
+        <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>218</v>
+      <c r="A5" s="21" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>219</v>
+      <c r="A6" s="21" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="17" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>245</v>
+      <c r="A12" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="22" t="s">
-        <v>252</v>
+      <c r="A13" s="21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="290">
   <si>
     <t>请求url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,608 +464,684 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, 群信息}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看单个群信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号、新密码、确认密码、[忘记密码时不添，登陆后修改密码需添写 ]（验证码，开发模式为9999）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置消息免打扰功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置系统提示音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取系统提示音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200, "text":状态}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200, "text":"ok"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status、groupid、userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态值（1/0）、群id、用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setNotRecieveMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setSysTipVoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, "text":"ok"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, x, y, width, height, degree, file</t>
+  </si>
+  <si>
+    <t>用户id、裁剪x,y,宽、高、角度、文件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":为1就是最终上传的头像名}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app可能会有出入，另做接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取七牛token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1, text:token}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存最后选择的头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,picname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,图片名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{code:0/1/-1, text:失败/成功/无参数}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取相册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!delUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!getUploadQiniuToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!getUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, targetid, type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, text:[好友位置]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取好友/群组地图坐标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交个人地理位置接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, latitude, longtitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id, 经度，纬度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, text:ok}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18，获取某人当前地理位置接口</t>
+  </si>
+  <si>
+    <t>17，提交个人地理位置接口</t>
+  </si>
+  <si>
+    <t>16，发起群聊接口</t>
+  </si>
+  <si>
+    <t>15，从群组踢出某人</t>
+  </si>
+  <si>
+    <t>14，添加人到群组</t>
+  </si>
+  <si>
+    <t>13，从我的常用联系人列表删除人的接口</t>
+  </si>
+  <si>
+    <t>12，添加人到我的常用联系人接口</t>
+  </si>
+  <si>
+    <t>11，获取group用户列表接口</t>
+  </si>
+  <si>
+    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
+  </si>
+  <si>
+    <t>9，设置群组信息接口</t>
+  </si>
+  <si>
+    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
+  </si>
+  <si>
+    <t>7，天坊公司组织结构数据接口</t>
+  </si>
+  <si>
+    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
+  </si>
+  <si>
+    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
+  </si>
+  <si>
+    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
+  </si>
+  <si>
+    <t>2，发送验证码接口，参数countrycode，mobile</t>
+  </si>
+  <si>
+    <t>1，登录接口</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!afterLogin</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!requestText</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!newPassword</t>
+  </si>
+  <si>
+    <t>friend!getMemberFriends</t>
+  </si>
+  <si>
+    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!groupList</t>
+  </si>
+  <si>
+    <t>group!groupInfo</t>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!listGroupMemebers</t>
+  </si>
+  <si>
+    <t>friend!addFriend</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend!delFriend</t>
+  </si>
+  <si>
+    <t>group!joinGroup</t>
+  </si>
+  <si>
+    <t>group!leftGroup</t>
+  </si>
+  <si>
+    <t>subLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map!getLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、增加修改群名称接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7、修改个人设置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8、联系人接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11、返回字段说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupids, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取群组列表（我加入的和我建的）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12、群信息群列表接口返回数据增加创建者对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(仅返回id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(返回成员数据)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群组id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,groupname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,新的群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13、同时添加多个好友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9、权限功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10、添加返回所有不是好友数据的接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增listGroupMembersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14、建群小灰条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、加入、退出、转移群接口bug查找。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除群全员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群成员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传,不传表示全员禁言)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传，不传表示全员解禁)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id，[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证app使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证web使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、userpwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（web端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,sex,email,phone,sign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、性别、email、电话、个人签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（app端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,email,mobile、phone、addredss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、邮箱、手机、电话、地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定是否存在好友关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getFriendsRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,friendid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,好友id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":"true"/"false"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,topid,toptype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id，置顶id，置顶类型(1群,2人)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群禁言状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>群id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"code":1, 群信息}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看单个群信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号、新密码、确认密码、[忘记密码时不添，登陆后修改密码需添写 ]（验证码，开发模式为9999）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置消息免打扰功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置系统提示音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取系统提示音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200, "text":状态}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200, "text":"ok"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>status、groupid、userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态值（1/0）、群id、用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setNotRecieveMsg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setSysTipVoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1, "text":"ok"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, x, y, width, height, degree, file</t>
-  </si>
-  <si>
-    <t>用户id、裁剪x,y,宽、高、角度、文件。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":为1就是最终上传的头像名}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>app可能会有出入，另做接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取七牛token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1, text:token}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存最后选择的头像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,picname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,图片名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{code:0/1/-1, text:失败/成功/无参数}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取相册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除头像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!delUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!getUploadQiniuToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!getUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, targetid, type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, text:[好友位置]}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取好友/群组地图坐标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提交个人地理位置接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, latitude, longtitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id, 经度，纬度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, text:ok}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18，获取某人当前地理位置接口</t>
-  </si>
-  <si>
-    <t>17，提交个人地理位置接口</t>
-  </si>
-  <si>
-    <t>16，发起群聊接口</t>
-  </si>
-  <si>
-    <t>15，从群组踢出某人</t>
-  </si>
-  <si>
-    <t>14，添加人到群组</t>
-  </si>
-  <si>
-    <t>13，从我的常用联系人列表删除人的接口</t>
-  </si>
-  <si>
-    <t>12，添加人到我的常用联系人接口</t>
-  </si>
-  <si>
-    <t>11，获取group用户列表接口</t>
-  </si>
-  <si>
-    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
-  </si>
-  <si>
-    <t>9，设置群组信息接口</t>
-  </si>
-  <si>
-    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
-  </si>
-  <si>
-    <t>7，天坊公司组织结构数据接口</t>
-  </si>
-  <si>
-    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
-  </si>
-  <si>
-    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
-  </si>
-  <si>
-    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
-  </si>
-  <si>
-    <t>2，发送验证码接口，参数countrycode，mobile</t>
-  </si>
-  <si>
-    <t>1，登录接口</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!afterLogin</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!requestText</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!newPassword</t>
-  </si>
-  <si>
-    <t>friend!getMemberFriends</t>
-  </si>
-  <si>
-    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!groupList</t>
-  </si>
-  <si>
-    <t>group!groupInfo</t>
-  </si>
-  <si>
-    <t>??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!listGroupMemebers</t>
-  </si>
-  <si>
-    <t>friend!addFriend</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>friend!delFriend</t>
-  </si>
-  <si>
-    <t>group!joinGroup</t>
-  </si>
-  <si>
-    <t>group!leftGroup</t>
-  </si>
-  <si>
-    <t>subLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map!getLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3、增加修改群名称接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7、修改个人设置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8、联系人接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11、返回字段说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupids, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取群组列表（我加入的和我建的）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12、群信息群列表接口返回数据增加创建者对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(仅返回id)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(返回成员数据)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群组id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,groupname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,新的群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13、同时添加多个好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9、权限功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10、添加返回所有不是好友数据的接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增listGroupMembersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14、建群小灰条</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5、加入、退出、转移群接口bug查找。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1,"text":}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解除群全员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群成员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传,不传表示全员禁言)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传，不传表示全员解禁)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id，[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证app使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证web使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、userpwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（web端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,sex,email,phone,sign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、性别、email、电话、个人签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（app端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,email,mobile、phone、addredss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、邮箱、手机、电话、地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupids</t>
+    <t>查询群禁言成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupMember</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1557,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1598,7 +1674,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -1619,7 +1695,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>104</v>
@@ -1639,16 +1715,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>9</v>
@@ -1688,10 +1764,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>28</v>
@@ -1709,13 +1785,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1739,16 +1815,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>261</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>12</v>
@@ -1758,16 +1834,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1781,7 +1857,7 @@
         <v>106</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>58</v>
@@ -1799,7 +1875,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>107</v>
@@ -1820,10 +1896,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>109</v>
@@ -1841,7 +1917,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
@@ -1862,7 +1938,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>36</v>
@@ -1878,31 +1954,31 @@
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="21.75" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>41</v>
+        <v>268</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>42</v>
+        <v>271</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>43</v>
+        <v>272</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>273</v>
+      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>42</v>
@@ -1911,64 +1987,64 @@
         <v>43</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>47</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>57</v>
@@ -1977,61 +2053,61 @@
         <v>58</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>270</v>
+        <v>64</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>78</v>
+        <v>250</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>267</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>72</v>
@@ -2039,54 +2115,54 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>213</v>
+        <v>78</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>86</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>86</v>
@@ -2096,435 +2172,531 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>190</v>
+        <v>71</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E30" s="6"/>
+        <v>221</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="6" t="s">
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E31" s="6"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>268</v>
+        <v>75</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>216</v>
+        <v>96</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="10" t="s">
+      <c r="E36" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="10"/>
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="6" t="s">
-        <v>225</v>
+        <v>114</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>112</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="6" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>245</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="E38" s="6"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>250</v>
-      </c>
       <c r="D39" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E39" s="6"/>
+        <v>248</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>243</v>
+      </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A40" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>72</v>
-      </c>
+    <row r="40" spans="1:7">
+      <c r="A40" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E40" s="6"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="A41" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>128</v>
+      <c r="A42" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>289</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>124</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E42" s="6"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="6"/>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A43" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11" t="s">
-        <v>133</v>
-      </c>
+      <c r="A44" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="11" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="6"/>
+        <v>201</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
-        <v>145</v>
+        <v>278</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>146</v>
+        <v>275</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>139</v>
+        <v>276</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="11" t="s">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>151</v>
+        <v>280</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>140</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E47" s="6"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>135</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="E48" s="6"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="11"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="6"/>
+      <c r="A49" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="G49" s="11" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="11"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="12" t="s">
+      <c r="B56" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C51" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="4"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A53" s="23" t="s">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A59" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A59:D59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2548,143 +2720,143 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" t="s">
         <v>183</v>
-      </c>
-      <c r="B6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2709,84 +2881,84 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
创建群组不在组中 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="435" windowWidth="14805" windowHeight="7680"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="接口" sheetId="1" r:id="rId1"/>
@@ -1364,10 +1364,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1671,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2714,7 +2714,7 @@
       <c r="A57" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="23" t="s">
         <v>233</v>
       </c>
       <c r="C57" s="11" t="s">
@@ -2748,12 +2748,12 @@
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
增加成员去重 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
地图、初始化 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="675" windowWidth="14805" windowHeight="7440"/>
+    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="接口" sheetId="1" r:id="rId1"/>
@@ -600,693 +600,693 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>{"code":-1/0/1, text:ok}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18，获取某人当前地理位置接口</t>
+  </si>
+  <si>
+    <t>17，提交个人地理位置接口</t>
+  </si>
+  <si>
+    <t>16，发起群聊接口</t>
+  </si>
+  <si>
+    <t>15，从群组踢出某人</t>
+  </si>
+  <si>
+    <t>14，添加人到群组</t>
+  </si>
+  <si>
+    <t>13，从我的常用联系人列表删除人的接口</t>
+  </si>
+  <si>
+    <t>12，添加人到我的常用联系人接口</t>
+  </si>
+  <si>
+    <t>11，获取group用户列表接口</t>
+  </si>
+  <si>
+    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
+  </si>
+  <si>
+    <t>9，设置群组信息接口</t>
+  </si>
+  <si>
+    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
+  </si>
+  <si>
+    <t>7，天坊公司组织结构数据接口</t>
+  </si>
+  <si>
+    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
+  </si>
+  <si>
+    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
+  </si>
+  <si>
+    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
+  </si>
+  <si>
+    <t>2，发送验证码接口，参数countrycode，mobile</t>
+  </si>
+  <si>
+    <t>1，登录接口</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!afterLogin</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!requestText</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system!newPassword</t>
+  </si>
+  <si>
+    <t>friend!getMemberFriends</t>
+  </si>
+  <si>
+    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!groupList</t>
+  </si>
+  <si>
+    <t>group!groupInfo</t>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group!listGroupMemebers</t>
+  </si>
+  <si>
+    <t>friend!addFriend</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend!delFriend</t>
+  </si>
+  <si>
+    <t>group!joinGroup</t>
+  </si>
+  <si>
+    <t>group!leftGroup</t>
+  </si>
+  <si>
+    <t>subLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map!getLocation</t>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、增加修改群名称接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7、修改个人设置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8、联系人接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11、返回字段说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取群组列表（我加入的和我建的）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1, "text":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12、群信息群列表接口返回数据增加创建者对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(仅返回id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群成员(返回成员数据)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群组id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,groupname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,新的群名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13、同时添加多个好友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9、权限功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10、添加返回所有不是好友数据的接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增listGroupMembersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14、建群小灰条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、加入、退出、转移群接口bug查找。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除群全员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群成员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传，不传表示全员解禁)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id，[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证app使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证web使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、userpwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（web端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（app端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,email,mobile、phone、addredss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、邮箱、手机、电话、地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定是否存在好友关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getFriendsRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,friendid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,好友id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":"true"/"false"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,topid,toptype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id，置顶id，置顶类型(1群,2人)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群禁言状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群禁言成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getNotRecieveMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息免打扰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid、userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id、用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!cancelMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>免登陆接口web端(必须用post提交)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>免登陆接口app端(必须用post提交)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branchId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有用户信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(非裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogoNotCut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证旧密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!valideOldPwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldpwd、accout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群在线人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getGroupOnLineMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取用户在线状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测单用户在线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,position,fullname,sex,email,phone,sign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有的职位信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传,不传表示全员禁言)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ｘ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id, 纬度，经度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>userid, latitude, longtitude</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"code":-1/0/1, text:ok}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18，获取某人当前地理位置接口</t>
-  </si>
-  <si>
-    <t>17，提交个人地理位置接口</t>
-  </si>
-  <si>
-    <t>16，发起群聊接口</t>
-  </si>
-  <si>
-    <t>15，从群组踢出某人</t>
-  </si>
-  <si>
-    <t>14，添加人到群组</t>
-  </si>
-  <si>
-    <t>13，从我的常用联系人列表删除人的接口</t>
-  </si>
-  <si>
-    <t>12，添加人到我的常用联系人接口</t>
-  </si>
-  <si>
-    <t>11，获取group用户列表接口</t>
-  </si>
-  <si>
-    <t>10，设置个人profile信息接口（目前主要是上传头像，设置地址，设置部门）</t>
-  </si>
-  <si>
-    <t>9，设置群组信息接口</t>
-  </si>
-  <si>
-    <t>8，获取群组信息接口，参数groupid，返回group信息，例如group名字，人数，创建时间，创建人，群组等</t>
-  </si>
-  <si>
-    <t>7，天坊公司组织结构数据接口</t>
-  </si>
-  <si>
-    <t>5，获取常用联系人列表接口，参数userid，返回［person,person,person...］</t>
-  </si>
-  <si>
-    <t>4，获取个人profile接口，参数userid，获取userid对应的person数据</t>
-  </si>
-  <si>
-    <t>3，重置密码接口，参数 mobile, verfiyCode，password</t>
-  </si>
-  <si>
-    <t>2，发送验证码接口，参数countrycode，mobile</t>
-  </si>
-  <si>
-    <t>1，登录接口</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!afterLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!afterLogin</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!testText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!requestText</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!newPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system!newPassword</t>
-  </si>
-  <si>
-    <t>friend!getMemberFriends</t>
-  </si>
-  <si>
-    <t>6，获取我的群组列表接口，参数userid，返回分两种：我建的群组[group,group...], 我加入的群组[group,group...]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!groupList</t>
-  </si>
-  <si>
-    <t>group!groupInfo</t>
-  </si>
-  <si>
-    <t>??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group!listGroupMemebers</t>
-  </si>
-  <si>
-    <t>friend!addFriend</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!delFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>friend!delFriend</t>
-  </si>
-  <si>
-    <t>group!joinGroup</t>
-  </si>
-  <si>
-    <t>group!leftGroup</t>
-  </si>
-  <si>
-    <t>subLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!getLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map!getLocation</t>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getSysTipVoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2、部门数据返回增加组织数据。数据拉直返回。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3、增加修改群名称接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4、群成员接口返回数据不要id，须返回所有群成员对象属性。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6、地图接口增加获取所有人和获取所有好友扩展。如果是这两个，targetId去掉或为0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7、修改个人设置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、群组列表接口返回数据须改为我建的群组和我加入的群组。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8、联系人接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11、返回字段说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取群组列表（我加入的和我建的）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1, "text":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12、群信息群列表接口返回数据增加创建者对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(仅返回id)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群成员(返回成员数据)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群组id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>修改群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,groupname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,新的群名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13、同时添加多个好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9、权限功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10、添加返回所有不是好友数据的接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增listGroupMembersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14、建群小灰条</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5、加入、退出、转移群接口bug查找。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1,"text":}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解除群全员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群成员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传，不传表示全员解禁)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id，[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证app使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证web使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、userpwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（web端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（app端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,email,mobile、phone、addredss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、邮箱、手机、电话、地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupids</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确定是否存在好友关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getFriendsRelation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,friendid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,好友id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1,"text":"true"/"false"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,topid,toptype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id，置顶id，置顶类型(1群,2人)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置消息置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取消息置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群禁言状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群禁言成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getNotRecieveMsg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取消息免打扰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid、userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id、用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>取消置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!cancelMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>免登陆接口web端(必须用post提交)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>免登陆接口app端(必须用post提交)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branchId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取所有用户信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(非裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogoNotCut</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证旧密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!valideOldPwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oldpwd、accout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群在线人数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getGroupOnLineMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取用户在线状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检测单用户在线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,position,fullname,sex,email,phone,sign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取所有的职位信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传,不传表示全员禁言)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ｘ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id, 纬度，经度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1294,7 +1294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2005,11 +2005,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="34.875" customWidth="1"/>
     <col min="2" max="2" width="73.875" customWidth="1"/>
@@ -2020,7 +2020,7 @@
     <col min="7" max="7" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2039,12 +2039,12 @@
       <c r="F1" s="3"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -2060,27 +2060,27 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>101</v>
@@ -2098,15 +2098,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>112</v>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -2147,12 +2147,12 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>27</v>
@@ -2168,27 +2168,27 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -2198,50 +2198,50 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="15" customFormat="1">
       <c r="A11" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="D11" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>281</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" s="15" customFormat="1">
       <c r="A12" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>282</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>283</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>241</v>
-      </c>
       <c r="C13" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>12</v>
@@ -2249,32 +2249,32 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>56</v>
@@ -2287,29 +2287,29 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>292</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>103</v>
@@ -2325,30 +2325,30 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>105</v>
@@ -2361,12 +2361,12 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>24</v>
@@ -2382,12 +2382,12 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>35</v>
@@ -2403,31 +2403,31 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>41</v>
@@ -2441,12 +2441,12 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>41</v>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>48</v>
@@ -2479,7 +2479,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2488,7 +2488,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -2526,9 +2526,9 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>61</v>
@@ -2545,15 +2545,15 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>74</v>
@@ -2564,12 +2564,12 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>75</v>
@@ -2583,12 +2583,12 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>75</v>
@@ -2600,7 +2600,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>67</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>68</v>
       </c>
@@ -2638,18 +2638,18 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>94</v>
@@ -2657,29 +2657,29 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>79</v>
@@ -2693,26 +2693,26 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7">
       <c r="A39" s="10" t="s">
         <v>84</v>
       </c>
@@ -2733,12 +2733,12 @@
       </c>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>91</v>
@@ -2752,7 +2752,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
         <v>97</v>
       </c>
@@ -2773,15 +2773,15 @@
       </c>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>246</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>247</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>108</v>
@@ -2792,113 +2792,113 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B44" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>229</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C46" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>321</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>323</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C47" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>266</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>307</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>308</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="12.75" customHeight="1">
       <c r="A49" s="10" t="s">
         <v>113</v>
       </c>
@@ -2917,35 +2917,35 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="15" customHeight="1">
       <c r="A50" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>273</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7">
       <c r="A51" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B51" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>189</v>
-      </c>
       <c r="D51" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>117</v>
@@ -2953,7 +2953,7 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7">
       <c r="A52" s="10" t="s">
         <v>115</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>122</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>114</v>
@@ -2972,63 +2972,63 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>259</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>261</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>262</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>276</v>
-      </c>
       <c r="C55" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>259</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>124</v>
@@ -3044,24 +3044,24 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" s="15" customFormat="1">
       <c r="A57" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="C57" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="B57" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="C57" s="23" t="s">
+      <c r="D57" s="23" t="s">
         <v>296</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>297</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="23"/>
       <c r="G57" s="23"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
         <v>135</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7">
       <c r="A59" s="10" t="s">
         <v>138</v>
       </c>
@@ -3095,12 +3095,12 @@
       <c r="F59" s="9"/>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7">
       <c r="A60" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>132</v>
@@ -3114,7 +3114,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7">
       <c r="A61" s="10" t="s">
         <v>128</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
@@ -3140,18 +3140,18 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7">
       <c r="A63" s="10" t="s">
         <v>144</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>142</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>143</v>
@@ -3159,26 +3159,26 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7">
       <c r="A64" s="11" t="s">
         <v>145</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C64" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7">
       <c r="A65" s="11"/>
       <c r="B65" s="22"/>
       <c r="C65" s="10"/>
@@ -3187,22 +3187,22 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7">
       <c r="A66" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>316</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>318</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="12"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7" ht="40.5" customHeight="1">
       <c r="A67" s="43" t="s">
         <v>23</v>
       </c>
@@ -3228,151 +3228,151 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="117.875" customWidth="1"/>
     <col min="2" max="2" width="37.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3389,92 +3389,92 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="75.875" customWidth="1"/>
     <col min="2" max="2" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>196</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="20" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="20" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="20" t="s">
-        <v>205</v>
-      </c>
       <c r="B12" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3492,12 +3492,12 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:12" ht="30.75" customHeight="1">
       <c r="B2" s="28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C2" s="29">
         <v>2</v>
@@ -3516,7 +3516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12" ht="29.25" customHeight="1">
       <c r="B3" s="31">
         <v>4</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="K3" s="35"/>
       <c r="L3" s="36"/>
     </row>
-    <row r="4" spans="2:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" ht="35.25" customHeight="1">
       <c r="B4" s="37"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -3550,7 +3550,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="39"/>
     </row>
-    <row r="5" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" ht="36.75" customHeight="1">
       <c r="B5" s="40"/>
       <c r="C5" s="27">
         <v>2</v>
@@ -3567,7 +3567,7 @@
       <c r="K5" s="35"/>
       <c r="L5" s="36"/>
     </row>
-    <row r="6" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12" ht="42" customHeight="1">
       <c r="B6" s="37"/>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -3584,7 +3584,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
     </row>
-    <row r="7" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12" ht="32.25" customHeight="1">
       <c r="B7" s="31"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
@@ -3599,7 +3599,7 @@
       <c r="K7" s="27"/>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12" ht="41.25" customHeight="1">
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="L8" s="39"/>
     </row>
-    <row r="9" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12" ht="38.25" customHeight="1">
       <c r="B9" s="40"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -3633,7 +3633,7 @@
       <c r="K9" s="35"/>
       <c r="L9" s="36"/>
     </row>
-    <row r="10" spans="2:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12" ht="39.75" customHeight="1">
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -3648,7 +3648,7 @@
       <c r="K10" s="38"/>
       <c r="L10" s="39"/>
     </row>
-    <row r="11" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12" ht="41.25" customHeight="1">
       <c r="B11" s="31">
         <v>7</v>
       </c>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="L11" s="36"/>
     </row>
-    <row r="12" spans="2:12" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="44.25" customHeight="1" thickBot="1">
       <c r="B12" s="33">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
验证 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -830,503 +830,503 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>account、friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13、同时添加多个好友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9、权限功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10、添加返回所有不是好友数据的接口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增listGroupMembersData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14、建群小灰条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、加入、退出、转移群接口bug查找。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除群全员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群成员禁言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传，不传表示全员解禁)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id,[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id，[用户id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证app使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证web使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、userpwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（web端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人设置信息保存（app端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,email,mobile、phone、addredss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、邮箱、手机、电话、地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定是否存在好友关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!getFriendsRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,friendid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,好友id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":-1/0/1,"text":"true"/"false"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!setMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,topid,toptype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id，置顶id，置顶类型(1群,2人)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群禁言状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群禁言成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!getNotRecieveMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取消息免打扰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid、userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群id、用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消置顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/fun!cancelMsgTop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>免登陆接口web端(必须用post提交)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>免登陆接口app端(必须用post提交)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branchId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有用户信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像(非裁剪)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogoNotCut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证旧密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/system!valideOldPwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldpwd、accout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询群在线人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!getGroupOnLineMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取用户在线状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测单用户在线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,position,fullname,sex,email,phone,sign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有的职位信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传,不传表示全员禁言)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ｘ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id, 纬度，经度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, targetid, type,isInit(可选参数，表示是否显示超时坐标90,180)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, latitude, longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以下是统一验证系统的接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取appId，和secret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置appId,secret,callbackUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/auth!getAppIDAndSecret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/auth!setAppIDAndSecretAndUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>appId,secret,url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200/500, text{appid,secret}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200/500, text:"OK/FAIL/ERROR"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/userservice!getToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13、同时添加多个好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9、权限功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10、添加返回所有不是好友数据的接口。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增listGroupMembersData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>web前端可能要做调整,调整群聊targetid为GID(已调整)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!joinGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14、建群小灰条</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5、加入、退出、转移群接口bug查找。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!transferGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!changeGroupName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!shutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1,"text":}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解除群全员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群成员禁言</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传，不传表示全员解禁)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id,[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id，[用户id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!createGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证app使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆验证web使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、userpwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!loginForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（web端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人设置信息保存（app端）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!updateMemberInfoForApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,email,mobile、phone、addredss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、邮箱、手机、电话、地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getBranchTreeAndMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupids</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确定是否存在好友关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getMemberFriends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!getFriendsRelation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,friendid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,好友id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":-1/0/1,"text":"true"/"false"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!setMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,topid,toptype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id，置顶id，置顶类型(1群,2人)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置消息置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取消息置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群禁言状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!unShutUpGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群禁言成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!getNotRecieveMsg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取消息免打扰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid、userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群id、用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>取消置顶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/fun!cancelMsgTop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!leftGroup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForWeb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!freeLandingForApp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!listGroupMemebers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>免登陆接口web端(必须用post提交)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>免登陆接口app端(必须用post提交)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branchId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account、newpwd、comparepwd、[oldpwd]（app端要多加这个textcode）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取所有用户信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getOneOfMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像(非裁剪)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!uploadUserLogoNotCut</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/upload!secUserLogos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证旧密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!requestText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/system!valideOldPwd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oldpwd、accout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查询群在线人数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getShutUpGroupMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!getGroupOnLineMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取用户在线状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检测单用户在线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,position,fullname,sex,email,phone,sign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取所有的职位信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传,不传表示全员禁言)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ｘ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id, 纬度，经度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, targetid, type,isInit(可选参数，表示是否显示超时坐标90,180)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, latitude, longitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>以下是统一验证系统的接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取appId，和secret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置appId,secret,callbackUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/auth!getAppIDAndSecret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/auth!setAppIDAndSecretAndUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>appId,secret,url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200/500, text{appid,secret}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200/500, text:"OK/FAIL/ERROR"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/userservice!getToken</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2091,7 +2091,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>299</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -2153,7 +2153,7 @@
         <v>167</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>111</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>163</v>
@@ -2217,13 +2217,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2235,7 +2235,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -2247,16 +2247,16 @@
     </row>
     <row r="11" spans="1:7" s="15" customFormat="1">
       <c r="A11" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="D11" s="23" t="s">
         <v>276</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>277</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
@@ -2264,13 +2264,13 @@
     </row>
     <row r="12" spans="1:7" s="15" customFormat="1">
       <c r="A12" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>278</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>279</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
@@ -2279,16 +2279,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>237</v>
-      </c>
       <c r="C13" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>12</v>
@@ -2298,16 +2298,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -2318,7 +2318,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>195</v>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>288</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2356,7 +2356,7 @@
         <v>101</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>102</v>
@@ -2374,13 +2374,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -2392,10 +2392,10 @@
         <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>104</v>
@@ -2434,7 +2434,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>35</v>
@@ -2452,19 +2452,19 @@
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
@@ -2474,7 +2474,7 @@
         <v>40</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>41</v>
@@ -2493,7 +2493,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>41</v>
@@ -2517,7 +2517,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>48</v>
@@ -2540,7 +2540,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>54</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>60</v>
@@ -2597,10 +2597,10 @@
         <v>63</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>73</v>
@@ -2616,7 +2616,7 @@
         <v>64</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>74</v>
@@ -2635,7 +2635,7 @@
         <v>65</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>74</v>
@@ -2690,7 +2690,7 @@
         <v>204</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>91</v>
@@ -2745,7 +2745,7 @@
         <v>198</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>199</v>
@@ -2785,7 +2785,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>90</v>
@@ -2825,10 +2825,10 @@
         <v>109</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>107</v>
@@ -2844,7 +2844,7 @@
         <v>208</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>209</v>
@@ -2858,35 +2858,35 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B44" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="9"/>
@@ -2894,35 +2894,35 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C46" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D46" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C47" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>262</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="9"/>
@@ -2930,16 +2930,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>303</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>304</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="9"/>
@@ -2966,16 +2966,16 @@
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1">
       <c r="A50" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>269</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>270</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="13"/>
@@ -3021,16 +3021,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>254</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>255</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="9"/>
@@ -3038,16 +3038,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>258</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="9"/>
@@ -3055,16 +3055,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>272</v>
-      </c>
       <c r="C55" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>254</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>255</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="9"/>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>123</v>
@@ -3093,16 +3093,16 @@
     </row>
     <row r="57" spans="1:7" s="15" customFormat="1">
       <c r="A57" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B57" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="C57" s="23" t="s">
+      <c r="D57" s="23" t="s">
         <v>292</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>293</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="23"/>
@@ -3147,7 +3147,7 @@
         <v>130</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>131</v>
@@ -3195,10 +3195,10 @@
         <v>183</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>141</v>
@@ -3211,13 +3211,13 @@
         <v>143</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>144</v>
@@ -3236,13 +3236,13 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>313</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="12"/>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="69" spans="1:7" ht="44.25" customHeight="1">
       <c r="A69" s="46" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B69" s="46"/>
       <c r="C69" s="46"/>
@@ -3280,36 +3280,36 @@
     </row>
     <row r="70" spans="1:7" ht="20.25" customHeight="1">
       <c r="A70" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B70" s="44" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D70" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>332</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>333</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7" ht="20.25" customHeight="1">
       <c r="A71" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B71" s="44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -3534,12 +3534,12 @@
         <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3559,12 +3559,12 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3577,17 +3577,17 @@
         <v>202</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3610,7 +3610,7 @@
     <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:12" ht="30.75" customHeight="1">
       <c r="B2" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C2" s="29">
         <v>2</v>

</xml_diff>

<commit_message>
oauth2登陆 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="765" windowWidth="14805" windowHeight="7350"/>
+    <workbookView xWindow="240" yWindow="795" windowWidth="14805" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="接口" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="问题" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
d Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/sealtalk/doc/接口协议.xlsx
+++ b/sealtalk/doc/接口协议.xlsx
@@ -1170,251 +1170,251 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取用户在线状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测单用户在线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid,position,fullname,sex,email,phone,sign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有的职位信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupid,userid(可不传,不传表示全员禁言)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, groupid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,群id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ｘ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id, 纬度，经度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, targetid, type,isInit(可选参数，表示是否显示超时坐标90,180)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid, latitude, longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取appId，和secret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置appId,secret,callbackUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/auth!getAppIDAndSecret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/auth!setAppIDAndSecretAndUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>appId,secret,url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200/500, text{appid,secret}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200/500, text:"OK/FAIL/ERROR"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/userservice!getToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景一取临时令牌</t>
+  </si>
+  <si>
+    <t>appId</t>
+  </si>
+  <si>
+    <t>场景二取临时令牌</t>
+  </si>
+  <si>
+    <t>unAuthToken，userName，userPwd，appId，info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景一登陆并授权，返回授权临时令牌</t>
+  </si>
+  <si>
+    <t>appId，unAuthToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景二授权</t>
+  </si>
+  <si>
+    <t>secret，authToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取访问令牌</t>
+  </si>
+  <si>
+    <t>visitToken</t>
+  </si>
+  <si>
+    <t>获取授权用户数据</t>
+  </si>
+  <si>
+    <t>模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已废弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辅助功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆相关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OAUTH2验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/getTempTokenSceneOne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/reqAuthorizeOne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/reqAuthorizeTwo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/getRealToken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/getAuthResource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%=request.getContextPath() %&gt;/getTempTokenSceneTwo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>&lt;%=request.getContextPath() %&gt;/group!getGroupOnLineMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取用户在线状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检测单用户在线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!searchUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/member!getAllMemberOnLineStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[userids]可选参数，传用户id组，不传表示全部用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid,position,fullname,sex,email,phone,sign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id、职位Id,全名，性别、email、电话、个人签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取所有的职位信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>groupid,userid(可不传,不传表示全员禁言)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, groupid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id,群id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":1/0,"text":1禁言，0非禁言}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ｘ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户id, 纬度，经度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/map!subLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身id，目标id（群组id/或好友id）,1是群组,2是单好友，3所有人，4所有好友(3，4targetId传0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, targetid, type,isInit(可选参数，表示是否显示超时坐标90,180)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid, latitude, longitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取appId，和secret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/branch!getPostion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置appId,secret,callbackUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/auth!getAppIDAndSecret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/auth!setAppIDAndSecretAndUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>appId,secret,url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200/500, text{appid,secret}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200/500, text:"OK/FAIL/ERROR"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/userservice!getToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/friend!addFriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/group!groupListWithAction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景一取临时令牌</t>
-  </si>
-  <si>
-    <t>appId</t>
-  </si>
-  <si>
-    <t>场景二取临时令牌</t>
-  </si>
-  <si>
-    <t>unAuthToken，userName，userPwd，appId，info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景一登陆并授权，返回授权临时令牌</t>
-  </si>
-  <si>
-    <t>appId，unAuthToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景二授权</t>
-  </si>
-  <si>
-    <t>secret，authToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取访问令牌</t>
-  </si>
-  <si>
-    <t>visitToken</t>
-  </si>
-  <si>
-    <t>获取授权用户数据</t>
-  </si>
-  <si>
-    <t>模块</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已废弃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>好友</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>群组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>辅助功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上传头像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>登陆相关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OAUTH2验证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/getTempTokenSceneOne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/reqAuthorizeOne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/reqAuthorizeTwo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/getRealToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/getAuthResource</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%=request.getContextPath() %&gt;/getTempTokenSceneTwo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1903,9 +1903,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1915,51 +1912,24 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1967,29 +1937,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1997,50 +1949,17 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2067,7 +1986,88 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2376,8 +2376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2393,8 +2393,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.5" customHeight="1">
-      <c r="A1" s="31" t="s">
-        <v>342</v>
+      <c r="A1" s="30" t="s">
+        <v>341</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2415,1340 +2415,1340 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="69" t="s">
+        <v>351</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="70"/>
+      <c r="B3" s="62" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="70"/>
+      <c r="B5" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="59"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="70"/>
+      <c r="B6" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="70"/>
+      <c r="B7" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="70"/>
+      <c r="B8" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="59"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="70"/>
+      <c r="B9" s="62" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="71"/>
+      <c r="B10" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="31" customFormat="1">
+      <c r="A11" s="77" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" s="31" customFormat="1">
+      <c r="A12" s="78"/>
+      <c r="B12" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="74" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="75"/>
+      <c r="B14" s="64" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="75"/>
+      <c r="B15" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="58"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="75"/>
+      <c r="B16" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="75"/>
+      <c r="B17" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="58"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="76"/>
+      <c r="B18" s="64" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>301</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>302</v>
+      </c>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="82" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="83"/>
+      <c r="B20" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="36"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="83"/>
+      <c r="B21" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="84"/>
+      <c r="B22" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="B2" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="84" t="s">
-        <v>291</v>
-      </c>
-      <c r="D2" s="84" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="84" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="84" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="84" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="84"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="85"/>
-      <c r="B3" s="89" t="s">
-        <v>290</v>
-      </c>
-      <c r="C3" s="84" t="s">
-        <v>292</v>
-      </c>
-      <c r="D3" s="84" t="s">
-        <v>293</v>
-      </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="90" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="84" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="85"/>
-      <c r="B5" s="89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="84" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="84" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5" s="84" t="s">
-        <v>111</v>
-      </c>
-      <c r="F5" s="84" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="84" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="84"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="85"/>
-      <c r="B6" s="89" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="85"/>
-      <c r="B7" s="89" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="85"/>
-      <c r="B8" s="89" t="s">
-        <v>227</v>
-      </c>
-      <c r="C8" s="84" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="84" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="84" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="84"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="85"/>
-      <c r="B9" s="89" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" s="84" t="s">
-        <v>230</v>
-      </c>
-      <c r="D9" s="84" t="s">
-        <v>229</v>
-      </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="86"/>
-      <c r="B10" s="89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="84" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="32" customFormat="1">
-      <c r="A11" s="36" t="s">
-        <v>344</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" s="32" customFormat="1">
-      <c r="A12" s="37"/>
-      <c r="B12" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>272</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="79" t="s">
-        <v>343</v>
-      </c>
-      <c r="B13" s="91" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" s="80" t="s">
-        <v>232</v>
-      </c>
-      <c r="D13" s="80" t="s">
-        <v>304</v>
-      </c>
-      <c r="E13" s="80" t="s">
-        <v>305</v>
-      </c>
-      <c r="F13" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="81"/>
-      <c r="B14" s="91" t="s">
-        <v>233</v>
-      </c>
-      <c r="C14" s="80" t="s">
-        <v>234</v>
-      </c>
-      <c r="D14" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="E14" s="80" t="s">
-        <v>236</v>
-      </c>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="81"/>
-      <c r="B15" s="91" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="80" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="80" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="80" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="80"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="81"/>
-      <c r="B16" s="91" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="80" t="s">
-        <v>281</v>
-      </c>
-      <c r="D16" s="80" t="s">
-        <v>282</v>
-      </c>
-      <c r="E16" s="80" t="s">
-        <v>282</v>
-      </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="81"/>
-      <c r="B17" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="80" t="s">
-        <v>301</v>
-      </c>
-      <c r="D17" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="80" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="80"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="82"/>
-      <c r="B18" s="91" t="s">
-        <v>299</v>
-      </c>
-      <c r="C18" s="80" t="s">
-        <v>302</v>
-      </c>
-      <c r="D18" s="80" t="s">
-        <v>303</v>
-      </c>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="38" t="s">
-        <v>346</v>
-      </c>
-      <c r="B19" s="95" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>217</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="41"/>
-      <c r="B20" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="40"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="41"/>
-      <c r="B21" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>319</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="42"/>
-      <c r="B22" s="95" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="96" t="s">
-        <v>353</v>
-      </c>
-      <c r="B23" s="53" t="s">
-        <v>318</v>
-      </c>
-      <c r="C23" s="53" t="s">
-        <v>321</v>
-      </c>
-      <c r="D23" s="53" t="s">
-        <v>323</v>
-      </c>
-      <c r="E23" s="53" t="s">
+      <c r="B23" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="F23" s="44" t="s">
         <v>325</v>
-      </c>
-      <c r="F23" s="53" t="s">
-        <v>326</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="96"/>
-      <c r="B24" s="53" t="s">
-        <v>320</v>
-      </c>
-      <c r="C24" s="53" t="s">
-        <v>322</v>
-      </c>
-      <c r="D24" s="53" t="s">
-        <v>324</v>
-      </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53" t="s">
-        <v>327</v>
+      <c r="A24" s="72"/>
+      <c r="B24" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44" t="s">
+        <v>326</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A25" s="96"/>
-      <c r="B25" s="52" t="s">
+      <c r="A25" s="72"/>
+      <c r="B25" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>331</v>
       </c>
-      <c r="C25" s="53" t="s">
-        <v>354</v>
-      </c>
-      <c r="D25" s="53" t="s">
-        <v>332</v>
-      </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A26" s="96"/>
-      <c r="B26" s="52" t="s">
-        <v>333</v>
-      </c>
-      <c r="C26" s="53" t="s">
-        <v>359</v>
-      </c>
-      <c r="D26" s="53" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="43" t="s">
         <v>332</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53"/>
+      <c r="C26" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="96"/>
-      <c r="B27" s="52" t="s">
-        <v>335</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>355</v>
-      </c>
-      <c r="D27" s="53" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="43" t="s">
         <v>334</v>
       </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="53"/>
+      <c r="C27" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A28" s="96"/>
-      <c r="B28" s="52" t="s">
-        <v>337</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="D28" s="53" t="s">
+      <c r="A28" s="72"/>
+      <c r="B28" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="E28" s="52"/>
-      <c r="F28" s="53"/>
+      <c r="C28" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="96"/>
-      <c r="B29" s="52" t="s">
-        <v>339</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>357</v>
-      </c>
-      <c r="D29" s="53" t="s">
+      <c r="A29" s="72"/>
+      <c r="B29" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
+      <c r="C29" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="96"/>
-      <c r="B30" s="52" t="s">
-        <v>341</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>358</v>
-      </c>
-      <c r="D30" s="53" t="s">
+      <c r="A30" s="72"/>
+      <c r="B30" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
+      <c r="C30" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="86"/>
+      <c r="B32" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="87"/>
+      <c r="B33" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="79" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="57"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="80"/>
+      <c r="B35" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="57"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A36" s="80"/>
+      <c r="B36" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="57"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1">
+      <c r="A37" s="81"/>
+      <c r="B37" s="65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>245</v>
+      </c>
+      <c r="F37" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="G37" s="67"/>
+      <c r="H37" s="57"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="88" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="57" t="s">
-        <v>328</v>
-      </c>
-      <c r="D31" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="57" t="s">
+      <c r="B38" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="89"/>
+      <c r="B39" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="D39" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A40" s="89"/>
+      <c r="B40" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>267</v>
+      </c>
+      <c r="D40" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="89"/>
+      <c r="B41" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="89"/>
+      <c r="B42" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="89"/>
+      <c r="B43" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="C43" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="D43" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="89"/>
+      <c r="B44" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="F44" s="53"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="89"/>
+      <c r="B45" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="89"/>
+      <c r="B46" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>329</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="59"/>
-      <c r="B33" s="55" t="s">
-        <v>300</v>
-      </c>
-      <c r="C33" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="75" t="s">
-        <v>345</v>
-      </c>
-      <c r="B34" s="92" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="76" t="s">
-        <v>329</v>
-      </c>
-      <c r="D34" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="76" t="s">
-        <v>104</v>
-      </c>
-      <c r="F34" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="93" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" s="76"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="77"/>
-      <c r="B35" s="92" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="76" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="H35" s="76"/>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A36" s="77"/>
-      <c r="B36" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="76" t="s">
-        <v>242</v>
-      </c>
-      <c r="D36" s="76" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="76" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="76"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
-      <c r="A37" s="78"/>
-      <c r="B37" s="92" t="s">
-        <v>241</v>
-      </c>
-      <c r="C37" s="76" t="s">
-        <v>243</v>
-      </c>
-      <c r="D37" s="76" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" s="76" t="s">
-        <v>245</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>246</v>
-      </c>
-      <c r="G37" s="94"/>
-      <c r="H37" s="76"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="66" t="s">
+      <c r="F46" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="89"/>
+      <c r="B47" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="H47" s="52"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="89"/>
+      <c r="B48" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="52" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="89"/>
+      <c r="B49" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="52"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="89"/>
+      <c r="B50" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="F50" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="89"/>
+      <c r="B51" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="D51" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="E51" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="F51" s="53"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="89"/>
+      <c r="B52" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="C52" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="E52" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="F52" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="89"/>
+      <c r="B53" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="C53" s="54" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E53" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="F53" s="53"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="89"/>
+      <c r="B54" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>260</v>
+      </c>
+      <c r="D54" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="E54" s="52" t="s">
+        <v>309</v>
+      </c>
+      <c r="F54" s="53" t="s">
+        <v>310</v>
+      </c>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="89"/>
+      <c r="B55" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>295</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E55" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="F55" s="53"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="90"/>
+      <c r="B56" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="C56" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="D56" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="E56" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="F56" s="53"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A57" s="91" t="s">
         <v>348</v>
       </c>
-      <c r="B38" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="68" t="s">
-        <v>226</v>
-      </c>
-      <c r="D38" s="68" t="s">
-        <v>240</v>
-      </c>
-      <c r="E38" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="69" t="s">
+      <c r="B57" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="70"/>
-      <c r="B39" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="68" t="s">
-        <v>213</v>
-      </c>
-      <c r="D39" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A40" s="70"/>
-      <c r="B40" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="68" t="s">
-        <v>267</v>
-      </c>
-      <c r="D40" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="70"/>
-      <c r="B41" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="70"/>
-      <c r="B42" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="70"/>
-      <c r="B43" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="C43" s="71" t="s">
-        <v>274</v>
-      </c>
-      <c r="D43" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="68" t="s">
-        <v>202</v>
-      </c>
-      <c r="F43" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="70"/>
-      <c r="B44" s="67" t="s">
-        <v>201</v>
-      </c>
-      <c r="C44" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="68" t="s">
-        <v>202</v>
-      </c>
-      <c r="F44" s="69"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="70"/>
-      <c r="B45" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="71" t="s">
-        <v>192</v>
-      </c>
-      <c r="D45" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="69" t="s">
-        <v>92</v>
-      </c>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="70"/>
-      <c r="B46" s="67" t="s">
-        <v>194</v>
-      </c>
-      <c r="C46" s="72" t="s">
-        <v>330</v>
-      </c>
-      <c r="D46" s="68" t="s">
-        <v>195</v>
-      </c>
-      <c r="E46" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="69" t="s">
-        <v>196</v>
-      </c>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="70"/>
-      <c r="B47" s="73" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="F47" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="H47" s="68"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="70"/>
-      <c r="B48" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="68" t="s">
-        <v>216</v>
-      </c>
-      <c r="D48" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="F48" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="70"/>
-      <c r="B49" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="69" t="s">
-        <v>97</v>
-      </c>
-      <c r="F49" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="G49" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="H49" s="68"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="70"/>
-      <c r="B50" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="71" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="68" t="s">
-        <v>238</v>
-      </c>
-      <c r="E50" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="70"/>
-      <c r="B51" s="67" t="s">
-        <v>204</v>
-      </c>
-      <c r="C51" s="71" t="s">
-        <v>218</v>
-      </c>
-      <c r="D51" s="68" t="s">
-        <v>205</v>
-      </c>
-      <c r="E51" s="68" t="s">
-        <v>206</v>
-      </c>
-      <c r="F51" s="69"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="70"/>
-      <c r="B52" s="67" t="s">
-        <v>222</v>
-      </c>
-      <c r="C52" s="71" t="s">
-        <v>219</v>
-      </c>
-      <c r="D52" s="68" t="s">
-        <v>308</v>
-      </c>
-      <c r="E52" s="68" t="s">
-        <v>224</v>
-      </c>
-      <c r="F52" s="69" t="s">
-        <v>220</v>
-      </c>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="70"/>
-      <c r="B53" s="67" t="s">
-        <v>221</v>
-      </c>
-      <c r="C53" s="71" t="s">
-        <v>254</v>
-      </c>
-      <c r="D53" s="68" t="s">
-        <v>223</v>
-      </c>
-      <c r="E53" s="68" t="s">
-        <v>225</v>
-      </c>
-      <c r="F53" s="69"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="70"/>
-      <c r="B54" s="67" t="s">
-        <v>253</v>
-      </c>
-      <c r="C54" s="71" t="s">
-        <v>260</v>
-      </c>
-      <c r="D54" s="68" t="s">
-        <v>309</v>
-      </c>
-      <c r="E54" s="68" t="s">
-        <v>310</v>
-      </c>
-      <c r="F54" s="69" t="s">
-        <v>311</v>
-      </c>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="70"/>
-      <c r="B55" s="67" t="s">
-        <v>257</v>
-      </c>
-      <c r="C55" s="71" t="s">
-        <v>295</v>
-      </c>
-      <c r="D55" s="68" t="s">
-        <v>255</v>
-      </c>
-      <c r="E55" s="68" t="s">
-        <v>256</v>
-      </c>
-      <c r="F55" s="69"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="74"/>
-      <c r="B56" s="67" t="s">
-        <v>294</v>
-      </c>
-      <c r="C56" s="71" t="s">
-        <v>296</v>
-      </c>
-      <c r="D56" s="68" t="s">
-        <v>297</v>
-      </c>
-      <c r="E56" s="68" t="s">
-        <v>298</v>
-      </c>
-      <c r="F56" s="69"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="68"/>
-    </row>
-    <row r="57" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A57" s="43" t="s">
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1">
+      <c r="A58" s="92"/>
+      <c r="B58" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="F58" s="42"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="92"/>
+      <c r="B59" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="92"/>
+      <c r="B60" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="92"/>
+      <c r="B61" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="E61" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="F61" s="39"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="92"/>
+      <c r="B62" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="F62" s="39"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="93"/>
+      <c r="B63" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="E63" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="F63" s="39"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="94" t="s">
         <v>349</v>
       </c>
-      <c r="B57" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E57" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-    </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1">
-      <c r="A58" s="47"/>
-      <c r="B58" s="48" t="s">
-        <v>262</v>
-      </c>
-      <c r="C58" s="49" t="s">
-        <v>261</v>
-      </c>
-      <c r="D58" s="49" t="s">
-        <v>263</v>
-      </c>
-      <c r="E58" s="49" t="s">
-        <v>264</v>
-      </c>
-      <c r="F58" s="50"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="47"/>
-      <c r="B59" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="D59" s="49" t="s">
-        <v>182</v>
-      </c>
-      <c r="E59" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="F59" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="47"/>
-      <c r="B60" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="E60" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="F60" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="47"/>
-      <c r="B61" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>248</v>
-      </c>
-      <c r="E61" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="F61" s="46"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="47"/>
-      <c r="B62" s="44" t="s">
-        <v>251</v>
-      </c>
-      <c r="C62" s="45" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="45" t="s">
-        <v>259</v>
-      </c>
-      <c r="E62" s="45" t="s">
-        <v>252</v>
-      </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="51"/>
-      <c r="B63" s="44" t="s">
-        <v>265</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="D63" s="45" t="s">
-        <v>248</v>
-      </c>
-      <c r="E63" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="F63" s="46"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="60" t="s">
-        <v>350</v>
-      </c>
-      <c r="B64" s="64" t="s">
+      <c r="B64" s="50" t="s">
         <v>284</v>
       </c>
-      <c r="C64" s="61" t="s">
+      <c r="C64" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="D64" s="61" t="s">
+      <c r="D64" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="E64" s="61" t="s">
+      <c r="E64" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="F64" s="62" t="s">
+      <c r="F64" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="G64" s="61"/>
-      <c r="H64" s="61" t="s">
+      <c r="G64" s="48"/>
+      <c r="H64" s="48" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="32" customFormat="1">
-      <c r="A65" s="63"/>
-      <c r="B65" s="64" t="s">
+    <row r="65" spans="1:8" s="31" customFormat="1">
+      <c r="A65" s="95"/>
+      <c r="B65" s="50" t="s">
         <v>285</v>
       </c>
-      <c r="C65" s="61" t="s">
+      <c r="C65" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="D65" s="61" t="s">
+      <c r="D65" s="48" t="s">
         <v>286</v>
       </c>
-      <c r="E65" s="61" t="s">
+      <c r="E65" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="F65" s="62"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="61"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="63"/>
-      <c r="B66" s="64" t="s">
+      <c r="A66" s="95"/>
+      <c r="B66" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="C66" s="61" t="s">
+      <c r="C66" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="D66" s="61" t="s">
+      <c r="D66" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="E66" s="61" t="s">
+      <c r="E66" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="F66" s="62"/>
-      <c r="G66" s="61"/>
-      <c r="H66" s="61"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="63"/>
-      <c r="B67" s="64" t="s">
+      <c r="A67" s="95"/>
+      <c r="B67" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="C67" s="61" t="s">
+      <c r="C67" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="61" t="s">
+      <c r="D67" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="E67" s="61" t="s">
+      <c r="E67" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="F67" s="62"/>
-      <c r="G67" s="61"/>
-      <c r="H67" s="61"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="65"/>
-      <c r="B68" s="64" t="s">
+      <c r="A68" s="96"/>
+      <c r="B68" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="61" t="s">
+      <c r="C68" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="D68" s="61" t="s">
+      <c r="D68" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="F68" s="62" t="s">
+      <c r="F68" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="G68" s="61"/>
-      <c r="H68" s="61"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="97" t="s">
-        <v>351</v>
-      </c>
-      <c r="B69" s="87" t="s">
+        <v>350</v>
+      </c>
+      <c r="B69" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="87" t="s">
+      <c r="C69" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="D69" s="87" t="s">
-        <v>316</v>
-      </c>
-      <c r="E69" s="87" t="s">
+      <c r="D69" s="60" t="s">
         <v>315</v>
       </c>
-      <c r="F69" s="88" t="s">
+      <c r="E69" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="F69" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="G69" s="87"/>
-      <c r="H69" s="87"/>
+      <c r="G69" s="60"/>
+      <c r="H69" s="60"/>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="97"/>
-      <c r="B70" s="87" t="s">
+      <c r="B70" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="87" t="s">
-        <v>314</v>
-      </c>
-      <c r="D70" s="87" t="s">
-        <v>317</v>
-      </c>
-      <c r="E70" s="87" t="s">
+      <c r="C70" s="60" t="s">
         <v>313</v>
       </c>
-      <c r="F70" s="88" t="s">
+      <c r="D70" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="E70" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="F70" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="G70" s="87"/>
-      <c r="H70" s="87"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="60"/>
     </row>
     <row r="71" spans="1:8" ht="20.25" customHeight="1">
       <c r="B71" s="4"/>
@@ -3759,12 +3759,12 @@
       <c r="H71" s="4"/>
     </row>
     <row r="72" spans="1:8" ht="40.5" customHeight="1">
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
+      <c r="E72" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4064,7 +4064,7 @@
     <row r="1" spans="2:12" ht="33.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:12" ht="30.75" customHeight="1">
       <c r="B2" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C2" s="15">
         <v>2</v>

</xml_diff>